<commit_message>
Added EquipmentManufacturer and EquipmentManufacturerModel to Equipment.dtsx
</commit_message>
<xml_diff>
--- a/Loading/EquipmentManufacturer/CurrentCycle/Data/EquipmentManufacturer - Template.xlsx
+++ b/Loading/EquipmentManufacturer/CurrentCycle/Data/EquipmentManufacturer - Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbuck\Documents\Projects\NNWW\AssetWorks Conversion\Loading\Equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\REPOS\AssetWorksConversion\Loading\EquipmentManufacturer\CurrentCycle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5784" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5784"/>
   </bookViews>
   <sheets>
     <sheet name="Manufacturer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Control</t>
   </si>
@@ -46,6 +46,33 @@
   </si>
   <si>
     <t>Model Name</t>
+  </si>
+  <si>
+    <t>[GROUPROW]</t>
+  </si>
+  <si>
+    <t>[KEY]</t>
+  </si>
+  <si>
+    <t>2134</t>
+  </si>
+  <si>
+    <t>532:02:00</t>
+  </si>
+  <si>
+    <t>534:02:00</t>
+  </si>
+  <si>
+    <t>534:14:00</t>
+  </si>
+  <si>
+    <t>534:06:00</t>
+  </si>
+  <si>
+    <t>534:07:00</t>
+  </si>
+  <si>
+    <t>534:16:00</t>
   </si>
 </sst>
 </file>
@@ -81,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,33 +391,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -399,34 +444,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>